<commit_message>
major rewrite! focus on testing :wink:
</commit_message>
<xml_diff>
--- a/tests/fixtures/simple.xlsx
+++ b/tests/fixtures/simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11020" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29300" windowHeight="18700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>FAMILY</t>
   </si>
@@ -48,15 +48,6 @@
     <t>ZF_7</t>
   </si>
   <si>
-    <t>rs10144418</t>
-  </si>
-  <si>
-    <t>rs1037256</t>
-  </si>
-  <si>
-    <t>rs1044973</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -66,15 +57,9 @@
     <t>T T</t>
   </si>
   <si>
-    <t>T C</t>
-  </si>
-  <si>
     <t>G G</t>
   </si>
   <si>
-    <t>C T</t>
-  </si>
-  <si>
     <t>A G</t>
   </si>
   <si>
@@ -85,16 +70,47 @@
   </si>
   <si>
     <t>ID-CG-000028T</t>
+  </si>
+  <si>
+    <t>ID-CG-000139T</t>
+  </si>
+  <si>
+    <t>rs9988021</t>
+  </si>
+  <si>
+    <t>rs115551684</t>
+  </si>
+  <si>
+    <t>rs199560653</t>
+  </si>
+  <si>
+    <t>G A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -117,14 +133,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -491,13 +531,13 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -505,37 +545,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -543,37 +583,37 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -581,41 +621,80 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" t="s">
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>